<commit_message>
Added Main with communication with DERTF
</commit_message>
<xml_diff>
--- a/utils/OPCUA/SetPointsData/MappaComandiTF_EMS_ConfigurazioneCentralizzata_AUTO.xlsx
+++ b/utils/OPCUA/SetPointsData/MappaComandiTF_EMS_ConfigurazioneCentralizzata_AUTO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/anderis_rse-web_it/Documents/Documenti/GitHub/ControlloDistribuito_DERTF/utils/Communication/OPCUA/SetPointsData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/polimeni_rse-web_it/Documents/Documenti/Tesi Magistrali/Polimi/OnlineLearning/utils/OPCUA/SetPointsData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="405" documentId="13_ncr:1_{C042575B-4D00-48DA-A1CB-7C21F6A04098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3C71F77-9000-4AB0-AEAB-FBA0ACBE88D8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S100" sheetId="5" r:id="rId1"/>
@@ -1022,7 +1022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1057,13 +1057,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1877,19 +1872,19 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="20.44140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -1909,7 +1904,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1927,7 +1922,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1945,7 +1940,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1964,7 +1959,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -1985,7 +1980,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>273</v>
       </c>
@@ -2003,7 +1998,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>166</v>
       </c>
@@ -2021,7 +2016,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>167</v>
       </c>
@@ -2039,7 +2034,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>11</v>
       </c>
@@ -2057,7 +2052,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>196</v>
       </c>
@@ -2077,15 +2072,15 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12"/>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13"/>
       <c r="D13"/>
     </row>
@@ -2127,18 +2122,18 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" customWidth="1"/>
-    <col min="4" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.88671875" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -2158,7 +2153,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>140</v>
       </c>
@@ -2176,7 +2171,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>178</v>
       </c>
@@ -2194,7 +2189,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>123</v>
       </c>
@@ -2212,7 +2207,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>127</v>
       </c>
@@ -2230,7 +2225,7 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>145</v>
       </c>
@@ -2248,7 +2243,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>182</v>
       </c>
@@ -2266,40 +2261,40 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
     </row>
   </sheetData>
@@ -2340,17 +2335,17 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.44140625" customWidth="1"/>
-    <col min="4" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="35.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -2370,7 +2365,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>267</v>
       </c>
@@ -2390,7 +2385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>268</v>
       </c>
@@ -2410,7 +2405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>269</v>
       </c>
@@ -2430,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2450,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>166</v>
       </c>
@@ -2470,7 +2465,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
@@ -2534,20 +2529,20 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="33.109375" customWidth="1"/>
-    <col min="4" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="35.88671875" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -2567,7 +2562,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2585,7 +2580,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2603,7 +2598,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -2624,7 +2619,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>166</v>
       </c>
@@ -2642,7 +2637,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>167</v>
       </c>
@@ -2660,7 +2655,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -2681,7 +2676,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2701,7 +2696,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -2719,7 +2714,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -2737,7 +2732,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -2757,7 +2752,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -2775,7 +2770,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>197</v>
       </c>
@@ -2795,10 +2790,10 @@
         <v>264</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="6"/>
     </row>
   </sheetData>
@@ -2857,18 +2852,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.44140625" customWidth="1"/>
-    <col min="2" max="2" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.109375" customWidth="1"/>
-    <col min="4" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.88671875" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -2888,7 +2883,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2907,7 +2902,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>42</v>
       </c>
@@ -2925,7 +2920,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>43</v>
       </c>
@@ -2943,7 +2938,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>46</v>
       </c>
@@ -2961,7 +2956,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>47</v>
       </c>
@@ -2979,7 +2974,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
@@ -2997,7 +2992,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>168</v>
       </c>
@@ -3015,7 +3010,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>169</v>
       </c>
@@ -3033,7 +3028,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>170</v>
       </c>
@@ -3051,7 +3046,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -3069,7 +3064,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -3087,7 +3082,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
@@ -3105,7 +3100,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>38</v>
       </c>
@@ -3123,7 +3118,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>39</v>
       </c>
@@ -3230,17 +3225,17 @@
       <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" customWidth="1"/>
-    <col min="2" max="2" width="45.88671875" customWidth="1"/>
-    <col min="3" max="3" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="35.88671875" customWidth="1"/>
+    <col min="7" max="7" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -3260,7 +3255,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>115</v>
       </c>
@@ -3278,7 +3273,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>116</v>
       </c>
@@ -3296,7 +3291,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>117</v>
       </c>
@@ -3314,7 +3309,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>118</v>
       </c>
@@ -3332,7 +3327,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>100</v>
       </c>
@@ -3352,7 +3347,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>102</v>
       </c>
@@ -3370,7 +3365,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>255</v>
       </c>
@@ -3388,7 +3383,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>256</v>
       </c>
@@ -3406,7 +3401,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>171</v>
       </c>
@@ -3424,7 +3419,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>172</v>
       </c>
@@ -3442,7 +3437,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>173</v>
       </c>
@@ -3460,7 +3455,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>174</v>
       </c>
@@ -3478,7 +3473,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>107</v>
       </c>
@@ -3496,7 +3491,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>184</v>
       </c>
@@ -3514,7 +3509,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>194</v>
       </c>
@@ -3532,7 +3527,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>262</v>
       </c>
@@ -3550,7 +3545,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>110</v>
       </c>
@@ -3568,7 +3563,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>195</v>
       </c>
@@ -3586,7 +3581,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -3604,7 +3599,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
@@ -3624,7 +3619,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
@@ -3642,7 +3637,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>60</v>
       </c>
@@ -3662,7 +3657,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>61</v>
       </c>
@@ -3680,7 +3675,7 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>62</v>
       </c>
@@ -3698,7 +3693,7 @@
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>63</v>
       </c>
@@ -3716,7 +3711,7 @@
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>64</v>
       </c>
@@ -3734,7 +3729,7 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>65</v>
       </c>
@@ -3752,7 +3747,7 @@
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>66</v>
       </c>
@@ -3770,7 +3765,7 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>59</v>
       </c>
@@ -3788,7 +3783,7 @@
       </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>67</v>
       </c>
@@ -3806,7 +3801,7 @@
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>57</v>
       </c>
@@ -3824,7 +3819,7 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>58</v>
       </c>
@@ -3842,7 +3837,7 @@
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
         <v>68</v>
       </c>
@@ -3860,7 +3855,7 @@
       </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>69</v>
       </c>
@@ -3878,7 +3873,7 @@
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>19</v>
       </c>
@@ -3896,7 +3891,7 @@
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>20</v>
       </c>
@@ -3914,7 +3909,7 @@
       </c>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
         <v>70</v>
       </c>
@@ -3932,7 +3927,7 @@
       </c>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>71</v>
       </c>
@@ -3950,7 +3945,7 @@
       </c>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
         <v>72</v>
       </c>
@@ -3968,7 +3963,7 @@
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
         <v>73</v>
       </c>
@@ -3986,7 +3981,7 @@
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
         <v>74</v>
       </c>
@@ -4004,7 +3999,7 @@
       </c>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
         <v>75</v>
       </c>
@@ -4022,7 +4017,7 @@
       </c>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
         <v>76</v>
       </c>
@@ -4040,7 +4035,7 @@
       </c>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>113</v>
       </c>
@@ -4098,24 +4093,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AEE9EB6-632C-481A-BC61-020C9E236F93}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1"/>
-    <col min="2" max="2" width="49.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -4135,7 +4130,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -4154,7 +4149,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -4175,11 +4170,11 @@
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>266</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -4193,14 +4188,14 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -4209,7 +4204,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>278</v>
       </c>
@@ -4225,7 +4220,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>201</v>
       </c>
@@ -4243,7 +4238,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>202</v>
       </c>
@@ -4261,7 +4256,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>204</v>
       </c>
@@ -4279,7 +4274,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>206</v>
       </c>
@@ -4297,7 +4292,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>208</v>
       </c>
@@ -4315,7 +4310,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>210</v>
       </c>
@@ -4333,7 +4328,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>211</v>
       </c>
@@ -4351,7 +4346,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>215</v>
       </c>
@@ -4369,7 +4364,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>217</v>
       </c>
@@ -4387,7 +4382,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>219</v>
       </c>
@@ -4405,7 +4400,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>221</v>
       </c>
@@ -4423,7 +4418,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>222</v>
       </c>
@@ -4441,7 +4436,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>223</v>
       </c>
@@ -4459,7 +4454,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>227</v>
       </c>
@@ -4476,9 +4471,8 @@
         <v>0</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="L20" s="18"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>228</v>
       </c>
@@ -4496,7 +4490,7 @@
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>229</v>
       </c>
@@ -4514,7 +4508,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>233</v>
       </c>
@@ -4532,7 +4526,7 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>234</v>
       </c>
@@ -4550,7 +4544,7 @@
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>237</v>
       </c>
@@ -4568,7 +4562,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -4586,7 +4580,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>239</v>
       </c>
@@ -4604,7 +4598,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>240</v>
       </c>
@@ -4622,7 +4616,7 @@
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>241</v>
       </c>
@@ -4640,7 +4634,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>245</v>
       </c>
@@ -4658,7 +4652,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>246</v>
       </c>
@@ -4676,7 +4670,7 @@
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>247</v>
       </c>
@@ -4694,7 +4688,7 @@
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>248</v>
       </c>
@@ -4712,7 +4706,7 @@
       </c>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>249</v>
       </c>
@@ -4732,7 +4726,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="C3:E4 D29:E1048576 C5">
+  <conditionalFormatting sqref="C3:E4 C5 D29:E1048576">
     <cfRule type="expression" dxfId="26" priority="2">
       <formula>C3="N"</formula>
     </cfRule>
@@ -4778,21 +4772,21 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" customWidth="1"/>
-    <col min="4" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.88671875" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -4812,7 +4806,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>137</v>
       </c>
@@ -4830,7 +4824,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>175</v>
       </c>
@@ -4848,7 +4842,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>120</v>
       </c>
@@ -4866,7 +4860,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>124</v>
       </c>
@@ -4884,7 +4878,7 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>142</v>
       </c>
@@ -4902,7 +4896,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>179</v>
       </c>
@@ -4920,40 +4914,40 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
     </row>
   </sheetData>
@@ -4991,22 +4985,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F32114F-D3B9-4AF6-B74A-C3E2C1F22211}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" customWidth="1"/>
-    <col min="4" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.88671875" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -5026,7 +5020,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>138</v>
       </c>
@@ -5044,7 +5038,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>176</v>
       </c>
@@ -5062,7 +5056,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>121</v>
       </c>
@@ -5080,7 +5074,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>125</v>
       </c>
@@ -5098,7 +5092,7 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>143</v>
       </c>
@@ -5116,7 +5110,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>180</v>
       </c>
@@ -5134,40 +5128,40 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
     </row>
   </sheetData>
@@ -5208,18 +5202,18 @@
       <selection activeCell="D5" sqref="D5:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" customWidth="1"/>
-    <col min="4" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.88671875" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -5239,7 +5233,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>139</v>
       </c>
@@ -5257,7 +5251,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>177</v>
       </c>
@@ -5275,7 +5269,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>122</v>
       </c>
@@ -5293,7 +5287,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>126</v>
       </c>
@@ -5311,7 +5305,7 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>144</v>
       </c>
@@ -5329,7 +5323,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>181</v>
       </c>
@@ -5347,40 +5341,40 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
     </row>
   </sheetData>
@@ -5414,6 +5408,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="41bcc58b-8f97-4aa7-8d6f-967843a37aea">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="efc33a24-6f18-474b-b279-7213570865a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9EE11730C39B04AA15158636D4E8287" ma:contentTypeVersion="18" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="844b771972d4ab5f116aeef8a5155c62">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="41bcc58b-8f97-4aa7-8d6f-967843a37aea" xmlns:ns3="efc33a24-6f18-474b-b279-7213570865a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="772b40f2ce67ed759c89bc187a89003e" ns2:_="" ns3:_="">
     <xsd:import namespace="41bcc58b-8f97-4aa7-8d6f-967843a37aea"/>
@@ -5662,27 +5676,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3A7F840-CE5B-44CB-8275-131FF951801A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="41bcc58b-8f97-4aa7-8d6f-967843a37aea"/>
+    <ds:schemaRef ds:uri="efc33a24-6f18-474b-b279-7213570865a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="41bcc58b-8f97-4aa7-8d6f-967843a37aea">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="efc33a24-6f18-474b-b279-7213570865a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34DA57F8-17BF-4606-BE62-FDAC2D6B20CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8178841-CB2A-438D-95AA-07D8986B8996}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5699,29 +5718,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34DA57F8-17BF-4606-BE62-FDAC2D6B20CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3A7F840-CE5B-44CB-8275-131FF951801A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="41bcc58b-8f97-4aa7-8d6f-967843a37aea"/>
-    <ds:schemaRef ds:uri="efc33a24-6f18-474b-b279-7213570865a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>